<commit_message>
Renaming all source and working directories in able to each user to share the project.
</commit_message>
<xml_diff>
--- a/Variables/Workforce Staff Codes.xlsx
+++ b/Variables/Workforce Staff Codes.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://healthsharedservice-my.sharepoint.com/personal/josh_andrews_dhsc_gov_uk/Documents/Nurse Data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://healthsharedservice-my.sharepoint.com/personal/josh_andrews_dhsc_gov_uk/Documents/Documents/R Codes/Workforce-Package/Variables/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="53" documentId="11_ACB6FFCE88992FF6D51F7302591EC3E3502CDD78" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{681C3DFD-0CA5-4307-BB80-15A391F183A8}"/>
+  <xr:revisionPtr revIDLastSave="187" documentId="11_ACB6FFCE88992FF6D51F7302591EC3E3502CDD78" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C1DDAE40-73A1-4C1E-A2DA-C0209928CCE1}"/>
   <bookViews>
-    <workbookView xWindow="-24120" yWindow="2445" windowWidth="24240" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="609" uniqueCount="608">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="706" uniqueCount="624">
   <si>
     <t>G0A</t>
   </si>
@@ -1844,6 +1844,54 @@
   </si>
   <si>
     <t>nurse_support_codes</t>
+  </si>
+  <si>
+    <t>nurse_adult_staff_codes</t>
+  </si>
+  <si>
+    <t>nurse_children_staff_codes</t>
+  </si>
+  <si>
+    <t>nurse_maternity_staff_codes</t>
+  </si>
+  <si>
+    <t>nurse_community_mental_health_staff_codes</t>
+  </si>
+  <si>
+    <t>nurse_other_mental_health_staff_codes</t>
+  </si>
+  <si>
+    <t>nurse_community_learning_difficulties_staff_codes</t>
+  </si>
+  <si>
+    <t>nurse_other_learning_difficulties_staff_codes</t>
+  </si>
+  <si>
+    <t>nurse_community_service_staff_codes</t>
+  </si>
+  <si>
+    <t>nurse_education_staff_codes</t>
+  </si>
+  <si>
+    <t>nurse_school_nursing_staff_codes</t>
+  </si>
+  <si>
+    <t>nurse_neonatal_staff_codes</t>
+  </si>
+  <si>
+    <t>N3J</t>
+  </si>
+  <si>
+    <t>nurse_learner_staff_codes</t>
+  </si>
+  <si>
+    <t>P1A</t>
+  </si>
+  <si>
+    <t>P1D</t>
+  </si>
+  <si>
+    <t>P1E</t>
   </si>
 </sst>
 </file>
@@ -2185,15 +2233,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Z80"/>
+  <dimension ref="A1:AL80"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="P13" sqref="P13:P33"/>
+    <sheetView tabSelected="1" topLeftCell="AD1" workbookViewId="0">
+      <selection activeCell="AF6" sqref="AF6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>566</v>
       </c>
@@ -2272,8 +2320,44 @@
       <c r="Z1" t="s">
         <v>590</v>
       </c>
-    </row>
-    <row r="2" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="AA1" t="s">
+        <v>608</v>
+      </c>
+      <c r="AB1" t="s">
+        <v>609</v>
+      </c>
+      <c r="AC1" t="s">
+        <v>610</v>
+      </c>
+      <c r="AD1" t="s">
+        <v>611</v>
+      </c>
+      <c r="AE1" t="s">
+        <v>612</v>
+      </c>
+      <c r="AF1" t="s">
+        <v>613</v>
+      </c>
+      <c r="AG1" t="s">
+        <v>614</v>
+      </c>
+      <c r="AH1" t="s">
+        <v>615</v>
+      </c>
+      <c r="AI1" t="s">
+        <v>616</v>
+      </c>
+      <c r="AJ1" t="s">
+        <v>617</v>
+      </c>
+      <c r="AK1" t="s">
+        <v>618</v>
+      </c>
+      <c r="AL1" t="s">
+        <v>620</v>
+      </c>
+    </row>
+    <row r="2" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -2352,8 +2436,44 @@
       <c r="Z2" t="s">
         <v>530</v>
       </c>
-    </row>
-    <row r="3" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="AA2" t="s">
+        <v>330</v>
+      </c>
+      <c r="AB2" t="s">
+        <v>331</v>
+      </c>
+      <c r="AC2" t="s">
+        <v>332</v>
+      </c>
+      <c r="AD2" t="s">
+        <v>333</v>
+      </c>
+      <c r="AE2" t="s">
+        <v>334</v>
+      </c>
+      <c r="AF2" t="s">
+        <v>335</v>
+      </c>
+      <c r="AG2" t="s">
+        <v>336</v>
+      </c>
+      <c r="AH2" t="s">
+        <v>337</v>
+      </c>
+      <c r="AI2" t="s">
+        <v>338</v>
+      </c>
+      <c r="AJ2" t="s">
+        <v>339</v>
+      </c>
+      <c r="AK2" t="s">
+        <v>340</v>
+      </c>
+      <c r="AL2" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="3" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -2429,8 +2549,44 @@
       <c r="Z3" t="s">
         <v>531</v>
       </c>
-    </row>
-    <row r="4" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="AA3" t="s">
+        <v>342</v>
+      </c>
+      <c r="AB3" t="s">
+        <v>343</v>
+      </c>
+      <c r="AC3" t="s">
+        <v>344</v>
+      </c>
+      <c r="AD3" t="s">
+        <v>345</v>
+      </c>
+      <c r="AE3" t="s">
+        <v>346</v>
+      </c>
+      <c r="AF3" t="s">
+        <v>347</v>
+      </c>
+      <c r="AG3" t="s">
+        <v>348</v>
+      </c>
+      <c r="AH3" t="s">
+        <v>349</v>
+      </c>
+      <c r="AI3" t="s">
+        <v>350</v>
+      </c>
+      <c r="AJ3" t="s">
+        <v>351</v>
+      </c>
+      <c r="AK3" t="s">
+        <v>352</v>
+      </c>
+      <c r="AL3" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="4" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -2506,8 +2662,44 @@
       <c r="Z4" t="s">
         <v>532</v>
       </c>
-    </row>
-    <row r="5" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="AA4" t="s">
+        <v>287</v>
+      </c>
+      <c r="AB4" t="s">
+        <v>288</v>
+      </c>
+      <c r="AC4" t="s">
+        <v>289</v>
+      </c>
+      <c r="AD4" t="s">
+        <v>290</v>
+      </c>
+      <c r="AE4" t="s">
+        <v>291</v>
+      </c>
+      <c r="AF4" t="s">
+        <v>291</v>
+      </c>
+      <c r="AG4" t="s">
+        <v>293</v>
+      </c>
+      <c r="AH4" t="s">
+        <v>353</v>
+      </c>
+      <c r="AI4" t="s">
+        <v>295</v>
+      </c>
+      <c r="AJ4" t="s">
+        <v>296</v>
+      </c>
+      <c r="AK4" t="s">
+        <v>297</v>
+      </c>
+      <c r="AL4" t="s">
+        <v>621</v>
+      </c>
+    </row>
+    <row r="5" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -2580,8 +2772,44 @@
       <c r="Z5" t="s">
         <v>533</v>
       </c>
-    </row>
-    <row r="6" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="AA5" t="s">
+        <v>309</v>
+      </c>
+      <c r="AB5" t="s">
+        <v>298</v>
+      </c>
+      <c r="AC5" t="s">
+        <v>299</v>
+      </c>
+      <c r="AD5" t="s">
+        <v>303</v>
+      </c>
+      <c r="AE5" t="s">
+        <v>313</v>
+      </c>
+      <c r="AF5" t="s">
+        <v>292</v>
+      </c>
+      <c r="AG5" t="s">
+        <v>315</v>
+      </c>
+      <c r="AH5" t="s">
+        <v>294</v>
+      </c>
+      <c r="AI5" t="s">
+        <v>301</v>
+      </c>
+      <c r="AJ5" t="s">
+        <v>341</v>
+      </c>
+      <c r="AK5" t="s">
+        <v>302</v>
+      </c>
+      <c r="AL5" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="6" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -2654,8 +2882,44 @@
       <c r="Z6" t="s">
         <v>534</v>
       </c>
-    </row>
-    <row r="7" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="AA6" t="s">
+        <v>320</v>
+      </c>
+      <c r="AB6" t="s">
+        <v>310</v>
+      </c>
+      <c r="AC6" t="s">
+        <v>284</v>
+      </c>
+      <c r="AD6" t="s">
+        <v>306</v>
+      </c>
+      <c r="AE6" t="s">
+        <v>324</v>
+      </c>
+      <c r="AF6" t="s">
+        <v>304</v>
+      </c>
+      <c r="AG6" t="s">
+        <v>326</v>
+      </c>
+      <c r="AH6" t="s">
+        <v>300</v>
+      </c>
+      <c r="AI6" t="s">
+        <v>619</v>
+      </c>
+      <c r="AJ6" t="s">
+        <v>318</v>
+      </c>
+      <c r="AK6" t="s">
+        <v>286</v>
+      </c>
+      <c r="AL6" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="7" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -2725,8 +2989,35 @@
       <c r="Z7" t="s">
         <v>535</v>
       </c>
-    </row>
-    <row r="8" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="AB7" t="s">
+        <v>321</v>
+      </c>
+      <c r="AC7" t="s">
+        <v>311</v>
+      </c>
+      <c r="AD7" t="s">
+        <v>312</v>
+      </c>
+      <c r="AF7" t="s">
+        <v>307</v>
+      </c>
+      <c r="AH7" t="s">
+        <v>579</v>
+      </c>
+      <c r="AI7" t="s">
+        <v>317</v>
+      </c>
+      <c r="AJ7" t="s">
+        <v>328</v>
+      </c>
+      <c r="AK7" t="s">
+        <v>319</v>
+      </c>
+      <c r="AL7" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="8" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -2793,8 +3084,29 @@
       <c r="Z8" t="s">
         <v>536</v>
       </c>
-    </row>
-    <row r="9" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="AC8" t="s">
+        <v>322</v>
+      </c>
+      <c r="AD8" t="s">
+        <v>323</v>
+      </c>
+      <c r="AF8" t="s">
+        <v>314</v>
+      </c>
+      <c r="AH8" t="s">
+        <v>305</v>
+      </c>
+      <c r="AI8" t="s">
+        <v>361</v>
+      </c>
+      <c r="AK8" t="s">
+        <v>329</v>
+      </c>
+      <c r="AL8" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="9" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -2858,8 +3170,17 @@
       <c r="Z9" t="s">
         <v>537</v>
       </c>
-    </row>
-    <row r="10" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="AF9" t="s">
+        <v>325</v>
+      </c>
+      <c r="AH9" t="s">
+        <v>308</v>
+      </c>
+      <c r="AL9" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="10" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>8</v>
       </c>
@@ -2923,8 +3244,14 @@
       <c r="Z10" t="s">
         <v>538</v>
       </c>
-    </row>
-    <row r="11" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="AH10" t="s">
+        <v>316</v>
+      </c>
+      <c r="AL10" t="s">
+        <v>622</v>
+      </c>
+    </row>
+    <row r="11" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>9</v>
       </c>
@@ -2988,8 +3315,14 @@
       <c r="Z11" t="s">
         <v>539</v>
       </c>
-    </row>
-    <row r="12" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="AH11" t="s">
+        <v>327</v>
+      </c>
+      <c r="AL11" t="s">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="12" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>10</v>
       </c>
@@ -3047,8 +3380,11 @@
       <c r="Z12" t="s">
         <v>540</v>
       </c>
-    </row>
-    <row r="13" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="AL12" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="13" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>11</v>
       </c>
@@ -3106,8 +3442,11 @@
       <c r="Z13" t="s">
         <v>541</v>
       </c>
-    </row>
-    <row r="14" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="AL13" t="s">
+        <v>623</v>
+      </c>
+    </row>
+    <row r="14" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>12</v>
       </c>
@@ -3157,7 +3496,7 @@
         <v>542</v>
       </c>
     </row>
-    <row r="15" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>13</v>
       </c>
@@ -3204,7 +3543,7 @@
         <v>543</v>
       </c>
     </row>
-    <row r="16" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>14</v>
       </c>

</xml_diff>